<commit_message>
fix/relocate longest and shortest path
</commit_message>
<xml_diff>
--- a/provat_qups1.xlsx
+++ b/provat_qups1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="1" state="visible" r:id="rId1"/>
@@ -1059,7 +1059,7 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:D8"/>
     </sheetView>
   </sheetViews>
@@ -1251,8 +1251,8 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1286,6 +1286,16 @@
           <t>Dhaka</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>মাধ্যমিক ও উচ্চমাধ্যমিক শিক্ষা বোর্ড, ঢাকা · 5 জয়নাগ রোড, ঢাকা</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ঢাকা</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1298,6 +1308,16 @@
           <t>University</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ইউনিভার্সিটি অব এশিয়া প্যাসিফিক | ইউএপি — বেসরকারি বিশ্ববিদ্যালয়, ঢাকা, বাংলাদেশ</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>University Of Dhaka</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1310,6 +1330,16 @@
           <t>Cricket</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>আন্তর্জাতিক ক্রিকেট কাউন্সিল — ক্রিকেট প্রশাসনিক সংস্থা</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>cricket</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1322,6 +1352,16 @@
           <t>Bombay</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>বোম্বে ভেলভেট — ২০১৫ সালের চলচ্চিত্র</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Bombay</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1334,6 +1374,16 @@
           <t>Football</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>football transfer news</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>football</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1346,6 +1396,16 @@
           <t>Paper</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>paper rhyme nikosh kalo ei adhare lyrics</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1356,6 +1416,16 @@
       <c r="B8" t="inlineStr">
         <is>
           <t>Knife</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>knife set price in bangladesh</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>knife</t>
         </is>
       </c>
     </row>

</xml_diff>